<commit_message>
Added Q3 (First Version)
</commit_message>
<xml_diff>
--- a/datasets/MarketData.xlsx
+++ b/datasets/MarketData.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Share\GianlucaPresario\CorsoCoripe\Coursework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shaani/Desktop/Shaan Ali/Bayes/Term 2 Modules/Fixed Income SMM269/Fixed Income Coursework/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55328B2A-4B91-46A0-A2A0-C488BEB4971D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E4D838-74CC-B24A-83C8-EACFDE05F631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="310" windowWidth="19420" windowHeight="9880" xr2:uid="{FF88EB87-1373-4D61-BE51-FCB3293BC599}"/>
+    <workbookView xWindow="6120" yWindow="500" windowWidth="29720" windowHeight="12960" xr2:uid="{FF88EB87-1373-4D61-BE51-FCB3293BC599}"/>
   </bookViews>
   <sheets>
-    <sheet name="Rates Deposits and IRS" sheetId="2" r:id="rId1"/>
-    <sheet name="shifted vol" sheetId="3" r:id="rId2"/>
-    <sheet name="cap premium" sheetId="4" r:id="rId3"/>
-    <sheet name="normal Vol" sheetId="5" r:id="rId4"/>
+    <sheet name="Deposit Rates" sheetId="2" r:id="rId1"/>
+    <sheet name="IRS Rates" sheetId="6" r:id="rId2"/>
+    <sheet name="shifted vol" sheetId="3" r:id="rId3"/>
+    <sheet name="cap premium" sheetId="4" r:id="rId4"/>
+    <sheet name="normal Vol" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -269,10 +270,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,441 +753,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D45725-F5A0-4004-BF05-F55897C2F7F6}">
-  <dimension ref="B2:J30"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="2">
+      <c r="B2">
         <v>3.1</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2.4119999999999999</v>
-      </c>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="2">
+      <c r="B3">
         <v>3.1</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2.218</v>
-      </c>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="2">
+      <c r="B4">
         <v>3.11</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2.202</v>
-      </c>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="2">
+      <c r="B5">
         <v>3.06</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="2">
-        <v>2.2120000000000002</v>
-      </c>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="2">
+      <c r="B6">
         <v>2.96</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2.2269999999999999</v>
-      </c>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="2">
+      <c r="B7">
         <v>2.73</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="2">
-        <v>2.2450000000000001</v>
-      </c>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="2">
+      <c r="B8">
         <v>2.66</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="2">
-        <v>2.2629999999999999</v>
-      </c>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="2">
+      <c r="B9">
         <v>2.5499999999999998</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="2">
-        <v>2.2839999999999998</v>
-      </c>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="2">
-        <v>2.306</v>
-      </c>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2.327</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="2">
-        <v>2.3460000000000001</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="2">
-        <v>2.3650000000000002</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="2">
-        <v>2.3809999999999998</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="2">
-        <v>2.3929999999999998</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="2">
-        <v>2.399</v>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="2">
-        <v>2.399</v>
-      </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="2">
-        <v>2.3940000000000001</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G20" s="2">
-        <v>2.383</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" s="2">
-        <v>2.3690000000000002</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="2">
-        <v>2.3530000000000002</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="2">
-        <v>2.2509999999999999</v>
-      </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" s="2">
-        <v>2.153</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="2">
-        <v>2.0670000000000002</v>
-      </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" s="2">
-        <v>1.988</v>
-      </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27" s="2">
-        <v>1.905</v>
-      </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" s="2">
-        <v>1.83</v>
-      </c>
-    </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="E29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G29" s="2">
-        <v>1.7210000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.35">
-      <c r="G30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1196,6 +845,329 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BF6D2F-3D32-624A-8F8F-055FF7603E2E}">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2">
+        <v>2.4119999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3">
+        <v>2.218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>2.202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>2.2120000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <v>2.2269999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>2.2450000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8">
+        <v>2.2629999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9">
+        <v>2.2839999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10">
+        <v>2.306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>2.327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>2.3460000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13">
+        <v>2.3650000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>2.3809999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15">
+        <v>2.3929999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16">
+        <v>2.399</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17">
+        <v>2.399</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18">
+        <v>2.3940000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>2.383</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20">
+        <v>2.3690000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21">
+        <v>2.3530000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>2.2509999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23">
+        <v>2.153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>2.0670000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25">
+        <v>1.988</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>1.905</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>1.7210000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B3F67A-D165-49F1-BD19-6B43663DFEB6}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1203,14 +1175,14 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F8BE84-F774-4112-AB80-0503AE2E7A04}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1218,14 +1190,14 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A87553B-048E-46E9-A818-609C15A84D74}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1233,7 +1205,7 @@
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>